<commit_message>
Testdata update for LIVEHTA-2532 and LIVEHTA-2534
</commit_message>
<xml_diff>
--- a/Testdata/Non_Oncology/DataFiles/ImportPublications/ImportPublicationsPage_Data.xlsx
+++ b/Testdata/Non_Oncology/DataFiles/ImportPublications/ImportPublicationsPage_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\Non_Oncology\DataFiles\ImportPublications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A445880-DD2D-41DB-863E-49293D291391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAC0654-4E6B-4280-9DB0-393F84894B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -241,9 +241,6 @@
     <t>Column ST-12 mapping key '_CustomData' is not supported. Only "EndpointResult_" is supported for arm-related data or "Extraction_" is supported for extraction-related data. Please modify accordingly and re-upload.</t>
   </si>
   <si>
-    <t>Column C-2 mapping key 'Ext_CustomData' is not supported. Only "Arm_" is supported for arm-related data or "Extraction_" is supported for extraction-related data. Please modify accordingly and re-upload.</t>
-  </si>
-  <si>
     <t>Column SE-3 mapping key 'A_CustomData' is not supported. Only "Arm_" is supported for arm-related data or "ExtractionEndpointInfo_" is supported for extraction-related data. Please modify accordingly and re-upload.</t>
   </si>
   <si>
@@ -283,9 +280,6 @@
     <t>Additional column found for 'QIIII', please re-check your template and upload again</t>
   </si>
   <si>
-    <t>In column 'CX' of the extraction file, variable label should be 'Timepoint unit' when the actual value is 'Invalid unit'</t>
-  </si>
-  <si>
     <t>Additional column found for 'T-2!@#$%', please re-check your template and upload again</t>
   </si>
   <si>
@@ -298,42 +292,21 @@
     <t>Additional column found for 'E-111', please re-check your template and upload again</t>
   </si>
   <si>
-    <t>In column 'BK' of the extraction file, variable label should be 'p-value' when the actual value is 'pvalue'</t>
-  </si>
-  <si>
     <t>Additional column found for 'QI-14', please re-check your template and upload again</t>
   </si>
   <si>
     <t>The extraction file is missing 'Add TTE Endpoint Custom Variables' and 'ST-12' as compared to the modified extraction template</t>
   </si>
   <si>
-    <t>In column 'BX' of the extraction file, variable label should be 'Add Endpoint overall results custom columns' when the actual value is 'Add Endpoint overall results custom colIvalidumns'</t>
-  </si>
-  <si>
     <t>Duplicate column found for QA-3, please re-check your template and upload again.</t>
   </si>
   <si>
-    <t>In column 'BR' of the extraction file, variable label should be 'Timepoint' when the actual value is 'Timepointssss'</t>
-  </si>
-  <si>
     <t>The extraction file is missing 'Add Endpoint overall results custom columns' and 'SO-3' as compared to the modified extraction template</t>
   </si>
   <si>
-    <t>In column 'CE' of the extraction file, variable ID should be 'RC-7' when the actual value is 'R-C-7'</t>
-  </si>
-  <si>
     <t>In column 'W' of the extraction file, variable label should be 'P-3' &amp; 'Add Variables for Treatment Characteristics' when the actual value is 'P-31' &amp; 'Invalid Add Variables for Treatment Characteristics'</t>
   </si>
   <si>
-    <t>In column 'AR' of the extraction file, variable label should be 'Add Endpoint Description custom columns' when the actual value is 'Invalid Col Name'</t>
-  </si>
-  <si>
-    <t>In column 'BU' of the extraction file, variable ID should be 'RI-5' when the actual value is 'RI-58'</t>
-  </si>
-  <si>
-    <t>In column 'BB' of the extraction file, variable label should be 'Number of events' when the actual value is '% of patients experiencing event'</t>
-  </si>
-  <si>
     <t>The extraction file is missing 'Safety N' and 'E-1' as compared to the modified extraction template</t>
   </si>
   <si>
@@ -349,12 +322,6 @@
     <t>\Testdata\Non_Oncology\Templates\ImportPublications\Extraction sheet - Invalid Data.xlsx</t>
   </si>
   <si>
-    <t>In column 'DK' of the extraction file, variable ID should be 'ST-9' when the actual value is '9-ST'</t>
-  </si>
-  <si>
-    <t>In column 'DP' of the extraction file, variable ID should be 'T-2' when the actual value is 'T-22'</t>
-  </si>
-  <si>
     <t>There is already an existing extraction file for LIVEHTA Automation - Test_NonOncology_Automation_1 , please remove the previous upload and re-upload.</t>
   </si>
   <si>
@@ -398,6 +365,39 @@
   </si>
   <si>
     <t>pop5</t>
+  </si>
+  <si>
+    <t>Column C-4 mapping key 'Ext_CustomData' is not supported. Only "Arm_" is supported for arm-related data or "Extraction_" is supported for extraction-related data. Please modify accordingly and re-upload.</t>
+  </si>
+  <si>
+    <t>In column 'AT' of the extraction file, variable label should be 'Add Endpoint Description custom columns' when the actual value is 'Invalid Col Name'</t>
+  </si>
+  <si>
+    <t>In column 'BD' of the extraction file, variable label should be 'Number of events' when the actual value is '% of patients experiencing event'</t>
+  </si>
+  <si>
+    <t>In column 'BM' of the extraction file, variable label should be 'p-value' when the actual value is 'pvalue'</t>
+  </si>
+  <si>
+    <t>In column 'BT' of the extraction file, variable label should be 'Timepoint' when the actual value is 'Timepointssss'</t>
+  </si>
+  <si>
+    <t>In column 'BW' of the extraction file, variable ID should be 'RI-5' when the actual value is 'RI-58'</t>
+  </si>
+  <si>
+    <t>In column 'BZ' of the extraction file, variable label should be 'Add Endpoint overall results custom columns' when the actual value is 'Add Endpoint overall results custom colIvalidumns'</t>
+  </si>
+  <si>
+    <t>In column 'CG' of the extraction file, variable ID should be 'RC-7' when the actual value is 'R-C-7'</t>
+  </si>
+  <si>
+    <t>In column 'CZ' of the extraction file, variable label should be 'Timepoint unit' when the actual value is 'Invalid unit'</t>
+  </si>
+  <si>
+    <t>In column 'DM' of the extraction file, variable ID should be 'ST-9' when the actual value is '9-ST'</t>
+  </si>
+  <si>
+    <t>In column 'DR' of the extraction file, variable ID should be 'T-2' when the actual value is 'T-22'</t>
   </si>
 </sst>
 </file>
@@ -727,9 +727,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B146" sqref="B146"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,7 +762,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -770,7 +770,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -779,7 +779,7 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -787,13 +787,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2">
         <v>4</v>
@@ -810,7 +810,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -821,7 +821,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -832,7 +832,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -843,7 +843,7 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -854,7 +854,7 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -865,7 +865,7 @@
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -876,7 +876,7 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -887,7 +887,7 @@
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -909,7 +909,7 @@
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -920,7 +920,7 @@
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -942,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -953,7 +953,7 @@
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -964,7 +964,7 @@
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -975,7 +975,7 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -997,7 +997,7 @@
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1008,7 +1008,7 @@
         <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1019,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1030,7 +1030,7 @@
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1041,7 +1041,7 @@
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1052,7 +1052,7 @@
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1085,7 +1085,7 @@
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1107,7 +1107,7 @@
         <v>5</v>
       </c>
       <c r="F32" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1118,7 +1118,7 @@
         <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1140,19 +1140,19 @@
         <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D36" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E36" s="2">
         <v>6</v>
       </c>
       <c r="F36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1163,7 +1163,7 @@
         <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1185,7 +1185,7 @@
         <v>6</v>
       </c>
       <c r="F39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1218,7 +1218,7 @@
         <v>6</v>
       </c>
       <c r="F42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1229,7 +1229,7 @@
         <v>6</v>
       </c>
       <c r="F43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1284,7 +1284,7 @@
         <v>6</v>
       </c>
       <c r="F48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1317,7 +1317,7 @@
         <v>6</v>
       </c>
       <c r="F51" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1339,7 +1339,7 @@
         <v>6</v>
       </c>
       <c r="F53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1361,7 +1361,7 @@
         <v>6</v>
       </c>
       <c r="F55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1372,13 +1372,13 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C57" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D57" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E57" s="2">
         <v>26</v>
@@ -2294,10 +2294,10 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B141" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
@@ -2309,117 +2309,117 @@
         <v>3</v>
       </c>
       <c r="F141" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E142" s="2">
         <v>11</v>
       </c>
       <c r="F142" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E143" s="2">
         <v>5</v>
       </c>
       <c r="F143" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E144" s="2">
         <v>13</v>
       </c>
       <c r="F144" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E145" s="2">
         <v>12</v>
       </c>
       <c r="F145" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E146" s="2">
         <v>4</v>
       </c>
       <c r="F146" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E147" s="2">
         <v>10</v>
       </c>
       <c r="F147" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E148" s="2">
         <v>9</v>
       </c>
       <c r="F148" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E149" s="2">
         <v>6</v>
       </c>
       <c r="F149" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E150" s="2">
         <v>8</v>
       </c>
       <c r="F150" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E151" s="2">
         <v>7</v>
       </c>
       <c r="F151" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>